<commit_message>
script can now output gilles.xlsm Todo: Implement User zu Windowsprinter and PC zu Default-Windowsprinter
</commit_message>
<xml_diff>
--- a/output/robot_printerserver_only_cari_relevant.xlsx
+++ b/output/robot_printerserver_only_cari_relevant.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:Q63"/>
+  <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,7 +521,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>PSTVA1629</t>
+          <t>PSTVA1730</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -531,17 +531,17 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>PSTVA1629-M0</t>
+          <t>PSTVA1730-M0</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>160.63.163.29</t>
+          <t>160.63.163.114</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>PSTVA1629</t>
+          <t>PSTVA1730</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
@@ -560,17 +560,17 @@
       </c>
       <c r="O2" t="inlineStr">
         <is>
-          <t>Canon iR-ADV C5760i</t>
+          <t>Brother HL-L6250DN</t>
         </is>
       </c>
       <c r="P2" t="inlineStr">
         <is>
-          <t>Canon Generic Plus PCL6</t>
+          <t>Brother HL-6250DN series</t>
         </is>
       </c>
       <c r="Q2" t="inlineStr">
         <is>
-          <t>DISPO</t>
+          <t>EG S04</t>
         </is>
       </c>
     </row>
@@ -587,7 +587,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>PSTVA1629</t>
+          <t>PSTVA1730</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -597,17 +597,17 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>PSTVA1629-S2</t>
+          <t>PSTVA1730-S2</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>160.63.163.29</t>
+          <t>160.63.163.114</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>PSTVA1629</t>
+          <t>PSTVA1730</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
@@ -626,17 +626,17 @@
       </c>
       <c r="O3" t="inlineStr">
         <is>
-          <t>Canon iR-ADV C5760i</t>
+          <t>Brother HL-L6250DN</t>
         </is>
       </c>
       <c r="P3" t="inlineStr">
         <is>
-          <t>Canon Generic Plus PCL6</t>
+          <t>Brother HL-6250DN series</t>
         </is>
       </c>
       <c r="Q3" t="inlineStr">
         <is>
-          <t>DISPO</t>
+          <t>EG S04</t>
         </is>
       </c>
     </row>
@@ -653,27 +653,27 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>PSTVA1639</t>
+          <t>PSTVA1731</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>M0</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>PSTVA1639-S2</t>
+          <t>PSTVA1731-M0</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>160.63.163.24</t>
+          <t>160.63.163.118</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>PSTVA1639</t>
+          <t>PSTVA1731</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
@@ -702,7 +702,7 @@
       </c>
       <c r="Q4" t="inlineStr">
         <is>
-          <t>AUK</t>
+          <t>EG S02</t>
         </is>
       </c>
     </row>
@@ -719,27 +719,27 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>PSTVA1639</t>
+          <t>PSTVA1731</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>S3</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>PSTVA1639-S3</t>
+          <t>PSTVA1731-S2</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>160.63.163.24</t>
+          <t>160.63.163.118</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>PSTVA1639</t>
+          <t>PSTVA1731</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
@@ -768,7 +768,7 @@
       </c>
       <c r="Q5" t="inlineStr">
         <is>
-          <t>AUK</t>
+          <t>EG S02</t>
         </is>
       </c>
     </row>
@@ -785,7 +785,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>PSTVA1688</t>
+          <t>PSTVA1732</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -795,17 +795,17 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>PSTVA1688-M0</t>
+          <t>PSTVA1732-M0</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>160.63.163.195</t>
+          <t>160.63.163.119</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>PSTVA1688</t>
+          <t>PSTVA1732</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
@@ -824,17 +824,17 @@
       </c>
       <c r="O6" t="inlineStr">
         <is>
-          <t>Canon iR-ADV C5540</t>
+          <t>Brother HL-L6250DN</t>
         </is>
       </c>
       <c r="P6" t="inlineStr">
         <is>
-          <t>Canon Generic Plus PCL6</t>
+          <t>Brother HL-6250DN series</t>
         </is>
       </c>
       <c r="Q6" t="inlineStr">
         <is>
-          <t>UG 1 B208</t>
+          <t>EG S03</t>
         </is>
       </c>
     </row>
@@ -851,27 +851,27 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>PSTVA1730</t>
+          <t>PSTVA1732</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>M0</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>PSTVA1730-M0</t>
+          <t>PSTVA1732-S2</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>160.63.163.114</t>
+          <t>160.63.163.119</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>PSTVA1730</t>
+          <t>PSTVA1732</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
@@ -900,7 +900,7 @@
       </c>
       <c r="Q7" t="inlineStr">
         <is>
-          <t>EG S04</t>
+          <t>EG S03</t>
         </is>
       </c>
     </row>
@@ -917,27 +917,27 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>PSTVA1730</t>
+          <t>PSTVA1733</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>M0</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>PSTVA1730-S2</t>
+          <t>PSTVA1733-M0</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>160.63.163.114</t>
+          <t>160.63.163.120</t>
         </is>
       </c>
       <c r="H8" t="inlineStr">
         <is>
-          <t>PSTVA1730</t>
+          <t>PSTVA1733</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
@@ -966,7 +966,7 @@
       </c>
       <c r="Q8" t="inlineStr">
         <is>
-          <t>EG S04</t>
+          <t>EG S05</t>
         </is>
       </c>
     </row>
@@ -983,27 +983,27 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>PSTVA1731</t>
+          <t>PSTVA1733</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>M0</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>PSTVA1731-M0</t>
+          <t>PSTVA1733-S2</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>160.63.163.118</t>
+          <t>160.63.163.120</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>PSTVA1731</t>
+          <t>PSTVA1733</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
@@ -1032,7 +1032,7 @@
       </c>
       <c r="Q9" t="inlineStr">
         <is>
-          <t>EG S02</t>
+          <t>EG S05</t>
         </is>
       </c>
     </row>
@@ -1049,7 +1049,7 @@
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>PSTVA1731</t>
+          <t>PSTVA1734</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -1059,17 +1059,17 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>PSTVA1731-S2</t>
+          <t>PSTVA1734-S2</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>160.63.163.118</t>
+          <t>160.63.163.121</t>
         </is>
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>PSTVA1731</t>
+          <t>PSTVA1734</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
@@ -1098,7 +1098,7 @@
       </c>
       <c r="Q10" t="inlineStr">
         <is>
-          <t>EG S02</t>
+          <t>EG S05</t>
         </is>
       </c>
     </row>
@@ -1115,27 +1115,27 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>PSTVA1732</t>
+          <t>PSTVA1735</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>M0</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>PSTVA1732-M0</t>
+          <t>PSTVA1735-S2</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>160.63.163.119</t>
+          <t>160.63.163.122</t>
         </is>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>PSTVA1732</t>
+          <t>PSTVA1735</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
@@ -1164,7 +1164,7 @@
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>EG S03</t>
+          <t>EG S05</t>
         </is>
       </c>
     </row>
@@ -1181,27 +1181,27 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>PSTVA1732</t>
+          <t>PSTVA1736</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>M0</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>PSTVA1732-S2</t>
+          <t>PSTVA1736-M0</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>160.63.163.119</t>
+          <t>160.63.163.123</t>
         </is>
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>PSTVA1732</t>
+          <t>PSTVA1736</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
@@ -1230,7 +1230,7 @@
       </c>
       <c r="Q12" t="inlineStr">
         <is>
-          <t>EG S03</t>
+          <t>EG S06</t>
         </is>
       </c>
     </row>
@@ -1247,27 +1247,27 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>PSTVA1733</t>
+          <t>PSTVA1736</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>M0</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>PSTVA1733-M0</t>
+          <t>PSTVA1736-S2</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>160.63.163.120</t>
+          <t>160.63.163.123</t>
         </is>
       </c>
       <c r="H13" t="inlineStr">
         <is>
-          <t>PSTVA1733</t>
+          <t>PSTVA1736</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
@@ -1296,7 +1296,7 @@
       </c>
       <c r="Q13" t="inlineStr">
         <is>
-          <t>EG S05</t>
+          <t>EG S06</t>
         </is>
       </c>
     </row>
@@ -1313,27 +1313,27 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>PSTVA1733</t>
+          <t>PSTVA1737</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>M0</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>PSTVA1733-S2</t>
+          <t>PSTVA1737-M0</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>160.63.163.120</t>
+          <t>160.63.163.124</t>
         </is>
       </c>
       <c r="H14" t="inlineStr">
         <is>
-          <t>PSTVA1733</t>
+          <t>PSTVA1737</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
@@ -1362,7 +1362,7 @@
       </c>
       <c r="Q14" t="inlineStr">
         <is>
-          <t>EG S05</t>
+          <t>EG S06</t>
         </is>
       </c>
     </row>
@@ -1379,32 +1379,32 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>PSTVA1734</t>
+          <t>PSTVA1737</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>PSTVA1734-S2</t>
+          <t>PSTVA1737-S1</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>160.63.163.121</t>
+          <t>160.63.163.124</t>
         </is>
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>PSTVA1734</t>
+          <t>PSTVA1737</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
@@ -1428,7 +1428,7 @@
       </c>
       <c r="Q15" t="inlineStr">
         <is>
-          <t>EG S05</t>
+          <t>EG S06</t>
         </is>
       </c>
     </row>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>PSTVA1735</t>
+          <t>PSTVA1737</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1455,17 +1455,17 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>PSTVA1735-S2</t>
+          <t>PSTVA1737-S2</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>160.63.163.122</t>
+          <t>160.63.163.124</t>
         </is>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>PSTVA1735</t>
+          <t>PSTVA1737</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
@@ -1494,7 +1494,7 @@
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>EG S05</t>
+          <t>EG S06</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>PSTVA1736</t>
+          <t>PSTVA1738</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1521,17 +1521,17 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>PSTVA1736-M0</t>
+          <t>PSTVA1738-M0</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>160.63.163.123</t>
+          <t>160.63.163.125</t>
         </is>
       </c>
       <c r="H17" t="inlineStr">
         <is>
-          <t>PSTVA1736</t>
+          <t>PSTVA1738</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
@@ -1560,7 +1560,7 @@
       </c>
       <c r="Q17" t="inlineStr">
         <is>
-          <t>EG S06</t>
+          <t>EG S07</t>
         </is>
       </c>
     </row>
@@ -1577,7 +1577,7 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>PSTVA1736</t>
+          <t>PSTVA1738</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1587,17 +1587,17 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>PSTVA1736-S2</t>
+          <t>PSTVA1738-S2</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>160.63.163.123</t>
+          <t>160.63.163.125</t>
         </is>
       </c>
       <c r="H18" t="inlineStr">
         <is>
-          <t>PSTVA1736</t>
+          <t>PSTVA1738</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
@@ -1626,7 +1626,7 @@
       </c>
       <c r="Q18" t="inlineStr">
         <is>
-          <t>EG S06</t>
+          <t>EG S07</t>
         </is>
       </c>
     </row>
@@ -1643,7 +1643,7 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>PSTVA1737</t>
+          <t>PSTVA1739</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1653,17 +1653,17 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>PSTVA1737-M0</t>
+          <t>PSTVA1739-M0</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>160.63.163.124</t>
+          <t>160.63.163.126</t>
         </is>
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>PSTVA1737</t>
+          <t>PSTVA1739</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
@@ -1692,7 +1692,7 @@
       </c>
       <c r="Q19" t="inlineStr">
         <is>
-          <t>EG S06</t>
+          <t>EG S07</t>
         </is>
       </c>
     </row>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>PSTVA1737</t>
+          <t>PSTVA1739</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1719,17 +1719,17 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>PSTVA1737-S1</t>
+          <t>PSTVA1739-S1</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>160.63.163.124</t>
+          <t>160.63.163.126</t>
         </is>
       </c>
       <c r="H20" t="inlineStr">
         <is>
-          <t>PSTVA1737</t>
+          <t>PSTVA1739</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
@@ -1758,7 +1758,7 @@
       </c>
       <c r="Q20" t="inlineStr">
         <is>
-          <t>EG S06</t>
+          <t>EG S07</t>
         </is>
       </c>
     </row>
@@ -1775,7 +1775,7 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>PSTVA1737</t>
+          <t>PSTVA1739</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1785,17 +1785,17 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>PSTVA1737-S2</t>
+          <t>PSTVA1739-S2</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>160.63.163.124</t>
+          <t>160.63.163.126</t>
         </is>
       </c>
       <c r="H21" t="inlineStr">
         <is>
-          <t>PSTVA1737</t>
+          <t>PSTVA1739</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
@@ -1824,7 +1824,7 @@
       </c>
       <c r="Q21" t="inlineStr">
         <is>
-          <t>EG S06</t>
+          <t>EG S07</t>
         </is>
       </c>
     </row>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>PSTVA1738</t>
+          <t>PSTVA1740</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1851,17 +1851,17 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>PSTVA1738-M0</t>
+          <t>PSTVA1740-M0</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>160.63.163.125</t>
+          <t>160.63.163.127</t>
         </is>
       </c>
       <c r="H22" t="inlineStr">
         <is>
-          <t>PSTVA1738</t>
+          <t>PSTVA1740</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
@@ -1890,7 +1890,7 @@
       </c>
       <c r="Q22" t="inlineStr">
         <is>
-          <t>EG S07</t>
+          <t>EG S08</t>
         </is>
       </c>
     </row>
@@ -1907,7 +1907,7 @@
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>PSTVA1738</t>
+          <t>PSTVA1740</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1917,17 +1917,17 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>PSTVA1738-S2</t>
+          <t>PSTVA1740-S2</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>160.63.163.125</t>
+          <t>160.63.163.127</t>
         </is>
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>PSTVA1738</t>
+          <t>PSTVA1740</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
@@ -1956,7 +1956,7 @@
       </c>
       <c r="Q23" t="inlineStr">
         <is>
-          <t>EG S07</t>
+          <t>EG S08</t>
         </is>
       </c>
     </row>
@@ -1973,7 +1973,7 @@
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>PSTVA1739</t>
+          <t>PSTVA1742</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1983,17 +1983,17 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>PSTVA1739-M0</t>
+          <t>PSTVA1742-M0</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>160.63.163.126</t>
+          <t>160.63.163.129</t>
         </is>
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>PSTVA1739</t>
+          <t>PSTVA1742</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
@@ -2022,7 +2022,7 @@
       </c>
       <c r="Q24" t="inlineStr">
         <is>
-          <t>EG S07</t>
+          <t>EG S08</t>
         </is>
       </c>
     </row>
@@ -2039,7 +2039,7 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>PSTVA1739</t>
+          <t>PSTVA1742</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -2049,17 +2049,17 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>PSTVA1739-S1</t>
+          <t>PSTVA1742-S1</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>160.63.163.126</t>
+          <t>160.63.163.129</t>
         </is>
       </c>
       <c r="H25" t="inlineStr">
         <is>
-          <t>PSTVA1739</t>
+          <t>PSTVA1742</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
@@ -2088,7 +2088,7 @@
       </c>
       <c r="Q25" t="inlineStr">
         <is>
-          <t>EG S07</t>
+          <t>EG S08</t>
         </is>
       </c>
     </row>
@@ -2105,7 +2105,7 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>PSTVA1739</t>
+          <t>PSTVA1742</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
@@ -2115,17 +2115,17 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>PSTVA1739-S2</t>
+          <t>PSTVA1742-S2</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>160.63.163.126</t>
+          <t>160.63.163.129</t>
         </is>
       </c>
       <c r="H26" t="inlineStr">
         <is>
-          <t>PSTVA1739</t>
+          <t>PSTVA1742</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
@@ -2154,7 +2154,7 @@
       </c>
       <c r="Q26" t="inlineStr">
         <is>
-          <t>EG S07</t>
+          <t>EG S08</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>PSTVA1740</t>
+          <t>PSTVA1743</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
@@ -2181,17 +2181,17 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>PSTVA1740-M0</t>
+          <t>PSTVA1743-M0</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>160.63.163.127</t>
+          <t>160.63.163.130</t>
         </is>
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>PSTVA1740</t>
+          <t>PSTVA1743</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
@@ -2220,7 +2220,7 @@
       </c>
       <c r="Q27" t="inlineStr">
         <is>
-          <t>EG S08</t>
+          <t>EG S09</t>
         </is>
       </c>
     </row>
@@ -2237,7 +2237,7 @@
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>PSTVA1740</t>
+          <t>PSTVA1743</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
@@ -2247,17 +2247,17 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>PSTVA1740-S2</t>
+          <t>PSTVA1743-S2</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>160.63.163.127</t>
+          <t>160.63.163.130</t>
         </is>
       </c>
       <c r="H28" t="inlineStr">
         <is>
-          <t>PSTVA1740</t>
+          <t>PSTVA1743</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
@@ -2286,7 +2286,7 @@
       </c>
       <c r="Q28" t="inlineStr">
         <is>
-          <t>EG S08</t>
+          <t>EG S09</t>
         </is>
       </c>
     </row>
@@ -2303,7 +2303,7 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>PSTVA1742</t>
+          <t>PSTVA1744</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
@@ -2313,17 +2313,17 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>PSTVA1742-M0</t>
+          <t>PSTVA1744-M0</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>160.63.163.129</t>
+          <t>160.63.163.131</t>
         </is>
       </c>
       <c r="H29" t="inlineStr">
         <is>
-          <t>PSTVA1742</t>
+          <t>PSTVA1744</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
@@ -2352,7 +2352,7 @@
       </c>
       <c r="Q29" t="inlineStr">
         <is>
-          <t>EG S08</t>
+          <t>EG S09</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>PSTVA1742</t>
+          <t>PSTVA1744</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
@@ -2379,17 +2379,17 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>PSTVA1742-S1</t>
+          <t>PSTVA1744-S1</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>160.63.163.129</t>
+          <t>160.63.163.131</t>
         </is>
       </c>
       <c r="H30" t="inlineStr">
         <is>
-          <t>PSTVA1742</t>
+          <t>PSTVA1744</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
@@ -2418,7 +2418,7 @@
       </c>
       <c r="Q30" t="inlineStr">
         <is>
-          <t>EG S08</t>
+          <t>EG S09</t>
         </is>
       </c>
     </row>
@@ -2435,7 +2435,7 @@
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>PSTVA1742</t>
+          <t>PSTVA1744</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -2445,17 +2445,17 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>PSTVA1742-S2</t>
+          <t>PSTVA1744-S2</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>160.63.163.129</t>
+          <t>160.63.163.131</t>
         </is>
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>PSTVA1742</t>
+          <t>PSTVA1744</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
@@ -2484,7 +2484,7 @@
       </c>
       <c r="Q31" t="inlineStr">
         <is>
-          <t>EG S08</t>
+          <t>EG S09</t>
         </is>
       </c>
     </row>
@@ -2501,7 +2501,7 @@
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>PSTVA1743</t>
+          <t>PSTVA1745</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -2511,17 +2511,17 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>PSTVA1743-M0</t>
+          <t>PSTVA1745-M0</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>160.63.163.130</t>
+          <t>160.63.163.132</t>
         </is>
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>PSTVA1743</t>
+          <t>PSTVA1745</t>
         </is>
       </c>
       <c r="J32" t="inlineStr">
@@ -2550,7 +2550,7 @@
       </c>
       <c r="Q32" t="inlineStr">
         <is>
-          <t>EG S09</t>
+          <t>EG S10</t>
         </is>
       </c>
     </row>
@@ -2567,27 +2567,27 @@
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>PSTVA1743</t>
+          <t>PSTVA1746</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>M0</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>PSTVA1743-S2</t>
+          <t>PSTVA1746-M0</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>160.63.163.130</t>
+          <t>160.63.163.133</t>
         </is>
       </c>
       <c r="H33" t="inlineStr">
         <is>
-          <t>PSTVA1743</t>
+          <t>PSTVA1746</t>
         </is>
       </c>
       <c r="J33" t="inlineStr">
@@ -2616,7 +2616,7 @@
       </c>
       <c r="Q33" t="inlineStr">
         <is>
-          <t>EG S09</t>
+          <t>EG S11</t>
         </is>
       </c>
     </row>
@@ -2633,27 +2633,27 @@
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>PSTVA1744</t>
+          <t>PSTVA1746</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>M0</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>PSTVA1744-M0</t>
+          <t>PSTVA1746-S2</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>160.63.163.131</t>
+          <t>160.63.163.133</t>
         </is>
       </c>
       <c r="H34" t="inlineStr">
         <is>
-          <t>PSTVA1744</t>
+          <t>PSTVA1746</t>
         </is>
       </c>
       <c r="J34" t="inlineStr">
@@ -2682,7 +2682,7 @@
       </c>
       <c r="Q34" t="inlineStr">
         <is>
-          <t>EG S09</t>
+          <t>EG S11</t>
         </is>
       </c>
     </row>
@@ -2699,32 +2699,32 @@
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>PSTVA1744</t>
+          <t>PSTVA1747</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>M0</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>PSTVA1744-S1</t>
+          <t>PSTVA1747-M0</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>160.63.163.131</t>
+          <t>160.63.163.134</t>
         </is>
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>PSTVA1744</t>
+          <t>PSTVA1747</t>
         </is>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A5</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
@@ -2748,7 +2748,7 @@
       </c>
       <c r="Q35" t="inlineStr">
         <is>
-          <t>EG S09</t>
+          <t>EG S08</t>
         </is>
       </c>
     </row>
@@ -2765,7 +2765,7 @@
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>PSTVA1744</t>
+          <t>PSTVA1747</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -2775,17 +2775,17 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>PSTVA1744-S2</t>
+          <t>PSTVA1747-S2</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>160.63.163.131</t>
+          <t>160.63.163.134</t>
         </is>
       </c>
       <c r="H36" t="inlineStr">
         <is>
-          <t>PSTVA1744</t>
+          <t>PSTVA1747</t>
         </is>
       </c>
       <c r="J36" t="inlineStr">
@@ -2814,7 +2814,7 @@
       </c>
       <c r="Q36" t="inlineStr">
         <is>
-          <t>EG S09</t>
+          <t>EG S08</t>
         </is>
       </c>
     </row>
@@ -2831,7 +2831,7 @@
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>PSTVA1745</t>
+          <t>PSTVA1763</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
@@ -2841,17 +2841,17 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>PSTVA1745-M0</t>
+          <t>PSTVA1763-M0</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>160.63.163.132</t>
+          <t>160.63.163.115</t>
         </is>
       </c>
       <c r="H37" t="inlineStr">
         <is>
-          <t>PSTVA1745</t>
+          <t>PSTVA1763</t>
         </is>
       </c>
       <c r="J37" t="inlineStr">
@@ -2880,7 +2880,7 @@
       </c>
       <c r="Q37" t="inlineStr">
         <is>
-          <t>EG S10</t>
+          <t>EG S02</t>
         </is>
       </c>
     </row>
@@ -2897,27 +2897,27 @@
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>PSTVA1746</t>
+          <t>PSTVA1763</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>M0</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>PSTVA1746-M0</t>
+          <t>PSTVA1763-S2</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>160.63.163.133</t>
+          <t>160.63.163.115</t>
         </is>
       </c>
       <c r="H38" t="inlineStr">
         <is>
-          <t>PSTVA1746</t>
+          <t>PSTVA1763</t>
         </is>
       </c>
       <c r="J38" t="inlineStr">
@@ -2946,7 +2946,7 @@
       </c>
       <c r="Q38" t="inlineStr">
         <is>
-          <t>EG S11</t>
+          <t>EG S02</t>
         </is>
       </c>
     </row>
@@ -2963,32 +2963,32 @@
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>PSTVA1746</t>
+          <t>PSTVA1764</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>S1</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>PSTVA1746-S2</t>
+          <t>PSTVA1764-S1</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>160.63.163.133</t>
+          <t>160.63.163.116</t>
         </is>
       </c>
       <c r="H39" t="inlineStr">
         <is>
-          <t>PSTVA1746</t>
+          <t>PSTVA1764</t>
         </is>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>A5</t>
+          <t>A4</t>
         </is>
       </c>
       <c r="K39" t="inlineStr">
@@ -3012,7 +3012,7 @@
       </c>
       <c r="Q39" t="inlineStr">
         <is>
-          <t>EG S11</t>
+          <t>EG S04</t>
         </is>
       </c>
     </row>
@@ -3029,27 +3029,27 @@
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>PSTVA1747</t>
+          <t>PSTVA1764</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>M0</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>PSTVA1747-M0</t>
+          <t>PSTVA1764-S2</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>160.63.163.134</t>
+          <t>160.63.163.116</t>
         </is>
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>PSTVA1747</t>
+          <t>PSTVA1764</t>
         </is>
       </c>
       <c r="J40" t="inlineStr">
@@ -3078,7 +3078,7 @@
       </c>
       <c r="Q40" t="inlineStr">
         <is>
-          <t>EG S08</t>
+          <t>EG S04</t>
         </is>
       </c>
     </row>
@@ -3095,27 +3095,27 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>PSTVA1747</t>
+          <t>PSTVA1765</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>M0</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>PSTVA1747-S2</t>
+          <t>PSTVA1765-M0</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>160.63.163.134</t>
+          <t>160.63.163.117</t>
         </is>
       </c>
       <c r="H41" t="inlineStr">
         <is>
-          <t>PSTVA1747</t>
+          <t>PSTVA1765</t>
         </is>
       </c>
       <c r="J41" t="inlineStr">
@@ -3144,7 +3144,7 @@
       </c>
       <c r="Q41" t="inlineStr">
         <is>
-          <t>EG S08</t>
+          <t>EG S14</t>
         </is>
       </c>
     </row>
@@ -3161,27 +3161,27 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>PSTVA1763</t>
+          <t>PSTVA1765</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>M0</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>PSTVA1763-M0</t>
+          <t>PSTVA1765-S2</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>160.63.163.115</t>
+          <t>160.63.163.117</t>
         </is>
       </c>
       <c r="H42" t="inlineStr">
         <is>
-          <t>PSTVA1763</t>
+          <t>PSTVA1765</t>
         </is>
       </c>
       <c r="J42" t="inlineStr">
@@ -3210,7 +3210,7 @@
       </c>
       <c r="Q42" t="inlineStr">
         <is>
-          <t>EG S02</t>
+          <t>EG S14</t>
         </is>
       </c>
     </row>
@@ -3227,27 +3227,27 @@
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>PSTVA1763</t>
+          <t>PSTVA1766</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>M0</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>PSTVA1763-S2</t>
+          <t>PSTVA1766-M0</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>160.63.163.115</t>
+          <t>160.63.163.153</t>
         </is>
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>PSTVA1763</t>
+          <t>PSTVA1766</t>
         </is>
       </c>
       <c r="J43" t="inlineStr">
@@ -3276,7 +3276,7 @@
       </c>
       <c r="Q43" t="inlineStr">
         <is>
-          <t>EG S02</t>
+          <t>EG S14</t>
         </is>
       </c>
     </row>
@@ -3293,32 +3293,32 @@
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>PSTVA1764</t>
+          <t>PSTVA1766</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>S1</t>
+          <t>S2</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>PSTVA1764-S1</t>
+          <t>PSTVA1766-S2</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>160.63.163.116</t>
+          <t>160.63.163.153</t>
         </is>
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>PSTVA1764</t>
+          <t>PSTVA1766</t>
         </is>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>A4</t>
+          <t>A5</t>
         </is>
       </c>
       <c r="K44" t="inlineStr">
@@ -3342,7 +3342,7 @@
       </c>
       <c r="Q44" t="inlineStr">
         <is>
-          <t>EG S04</t>
+          <t>EG S14</t>
         </is>
       </c>
     </row>
@@ -3359,7 +3359,7 @@
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>PSTVA1764</t>
+          <t>PSTVA1769</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -3369,17 +3369,17 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>PSTVA1764-S2</t>
+          <t>PSTVA1769-S2</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
         <is>
-          <t>160.63.163.116</t>
+          <t>160.63.163.154</t>
         </is>
       </c>
       <c r="H45" t="inlineStr">
         <is>
-          <t>PSTVA1764</t>
+          <t>PSTVA1769</t>
         </is>
       </c>
       <c r="J45" t="inlineStr">
@@ -3398,17 +3398,17 @@
       </c>
       <c r="O45" t="inlineStr">
         <is>
-          <t>Brother HL-L6250DN</t>
+          <t>Canon iR-ADV C5540</t>
         </is>
       </c>
       <c r="P45" t="inlineStr">
         <is>
-          <t>Brother HL-6250DN series</t>
+          <t>Canon Generic Plus PCL6</t>
         </is>
       </c>
       <c r="Q45" t="inlineStr">
         <is>
-          <t>EG S04</t>
+          <t>EG S21</t>
         </is>
       </c>
     </row>
@@ -3425,27 +3425,27 @@
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>PSTVA1765</t>
+          <t>PSTVA1769</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>M0</t>
+          <t>S3</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>PSTVA1765-M0</t>
+          <t>PSTVA1769-S3</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
         <is>
-          <t>160.63.163.117</t>
+          <t>160.63.163.154</t>
         </is>
       </c>
       <c r="H46" t="inlineStr">
         <is>
-          <t>PSTVA1765</t>
+          <t>PSTVA1769</t>
         </is>
       </c>
       <c r="J46" t="inlineStr">
@@ -3464,24 +3464,24 @@
       </c>
       <c r="O46" t="inlineStr">
         <is>
-          <t>Brother HL-L6250DN</t>
+          <t>Canon iR-ADV C5540</t>
         </is>
       </c>
       <c r="P46" t="inlineStr">
         <is>
-          <t>Brother HL-6250DN series</t>
+          <t>Canon Generic Plus PCL6</t>
         </is>
       </c>
       <c r="Q46" t="inlineStr">
         <is>
-          <t>EG S14</t>
+          <t>EG S21</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>AL</t>
+          <t>LE</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
@@ -3491,27 +3491,27 @@
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>PSTVA1765</t>
+          <t>PSTVA3199</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>S2</t>
+          <t>S4</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>PSTVA1765-S2</t>
+          <t>PSTVA3199-S4</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
         <is>
-          <t>160.63.163.117</t>
+          <t>160.63.178.99</t>
         </is>
       </c>
       <c r="H47" t="inlineStr">
         <is>
-          <t>PSTVA1765</t>
+          <t>PSTVA3199</t>
         </is>
       </c>
       <c r="J47" t="inlineStr">
@@ -3538,1064 +3538,8 @@
           <t>Brother HL-6250DN series</t>
         </is>
       </c>
-      <c r="Q47" t="inlineStr">
-        <is>
-          <t>EG S14</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>AL</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>PSTVA1766</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>M0</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>PSTVA1766-M0</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>160.63.163.153</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>PSTVA1766</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K48" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr"/>
-      <c r="N48" t="n">
-        <v>1</v>
-      </c>
-      <c r="O48" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P48" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q48" t="inlineStr">
-        <is>
-          <t>EG S14</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>AL</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D49" t="inlineStr">
-        <is>
-          <t>PSTVA1766</t>
-        </is>
-      </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>PSTVA1766-S2</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>160.63.163.153</t>
-        </is>
-      </c>
-      <c r="H49" t="inlineStr">
-        <is>
-          <t>PSTVA1766</t>
-        </is>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K49" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr"/>
-      <c r="N49" t="n">
-        <v>1</v>
-      </c>
-      <c r="O49" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P49" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q49" t="inlineStr">
-        <is>
-          <t>EG S14</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>AL</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>PSTVA1769</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>PSTVA1769-S2</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>160.63.163.154</t>
-        </is>
-      </c>
-      <c r="H50" t="inlineStr">
-        <is>
-          <t>PSTVA1769</t>
-        </is>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K50" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr"/>
-      <c r="N50" t="n">
-        <v>1</v>
-      </c>
-      <c r="O50" t="inlineStr">
-        <is>
-          <t>Canon iR-ADV C5540</t>
-        </is>
-      </c>
-      <c r="P50" t="inlineStr">
-        <is>
-          <t>Canon Generic Plus PCL6</t>
-        </is>
-      </c>
-      <c r="Q50" t="inlineStr">
-        <is>
-          <t>EG S21</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>AL</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D51" t="inlineStr">
-        <is>
-          <t>PSTVA1769</t>
-        </is>
-      </c>
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>PSTVA1769-S3</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>160.63.163.154</t>
-        </is>
-      </c>
-      <c r="H51" t="inlineStr">
-        <is>
-          <t>PSTVA1769</t>
-        </is>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K51" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr"/>
-      <c r="N51" t="n">
-        <v>1</v>
-      </c>
-      <c r="O51" t="inlineStr">
-        <is>
-          <t>Canon iR-ADV C5540</t>
-        </is>
-      </c>
-      <c r="P51" t="inlineStr">
-        <is>
-          <t>Canon Generic Plus PCL6</t>
-        </is>
-      </c>
-      <c r="Q51" t="inlineStr">
-        <is>
-          <t>EG S21</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>WI</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D52" t="inlineStr">
-        <is>
-          <t>PSTVA2600</t>
-        </is>
-      </c>
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>M0</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>PSTVA2600-M0</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>160.63.170.33</t>
-        </is>
-      </c>
-      <c r="H52" t="inlineStr">
-        <is>
-          <t>PSTVA2600</t>
-        </is>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K52" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr"/>
-      <c r="N52" t="n">
-        <v>1</v>
-      </c>
-      <c r="O52" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P52" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q52" t="inlineStr">
-        <is>
-          <t>EG S11</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>WI</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D53" t="inlineStr">
-        <is>
-          <t>PSTVA2629</t>
-        </is>
-      </c>
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>PSTVA2629-S2</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>160.63.170.27</t>
-        </is>
-      </c>
-      <c r="H53" t="inlineStr">
-        <is>
-          <t>PSTVA2629</t>
-        </is>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K53" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr"/>
-      <c r="N53" t="n">
-        <v>1</v>
-      </c>
-      <c r="O53" t="inlineStr">
-        <is>
-          <t>Canon iR-ADV C5540</t>
-        </is>
-      </c>
-      <c r="P53" t="inlineStr">
-        <is>
-          <t>Canon Generic Plus PCL6</t>
-        </is>
-      </c>
-      <c r="Q53" t="inlineStr">
-        <is>
-          <t>EG Dispo</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>WI</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>PSTVA2679</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>M0</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>PSTVA2679-M0</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>160.63.170.39</t>
-        </is>
-      </c>
-      <c r="H54" t="inlineStr">
-        <is>
-          <t>PSTVA2679</t>
-        </is>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K54" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr"/>
-      <c r="N54" t="n">
-        <v>1</v>
-      </c>
-      <c r="O54" t="inlineStr">
-        <is>
-          <t>Canon iR-ADV C5540</t>
-        </is>
-      </c>
-      <c r="P54" t="inlineStr">
-        <is>
-          <t>Canon Generic Plus PCL6</t>
-        </is>
-      </c>
-      <c r="Q54" t="inlineStr">
-        <is>
-          <t>PH B065</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>LE</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D55" t="inlineStr">
-        <is>
-          <t>PSTVA3199</t>
-        </is>
-      </c>
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>S4</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>PSTVA3199-S4</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>160.63.178.99</t>
-        </is>
-      </c>
-      <c r="H55" t="inlineStr">
-        <is>
-          <t>PSTVA3199</t>
-        </is>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K55" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr"/>
-      <c r="N55" t="n">
-        <v>1</v>
-      </c>
-      <c r="O55" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P55" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q55" t="n">
+      <c r="Q47" t="n">
         <v/>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>RE</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>PSTVA4670</t>
-        </is>
-      </c>
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>PSTVA4670-S2</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>160.63.179.15</t>
-        </is>
-      </c>
-      <c r="H56" t="inlineStr">
-        <is>
-          <t>PSTVA4670</t>
-        </is>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K56" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr"/>
-      <c r="N56" t="n">
-        <v>1</v>
-      </c>
-      <c r="O56" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P56" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q56" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EG Experten </t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>RE</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>PSTVA4670</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>PSTVA4670-S3</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>160.63.179.15</t>
-        </is>
-      </c>
-      <c r="H57" t="inlineStr">
-        <is>
-          <t>PSTVA4670</t>
-        </is>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K57" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr"/>
-      <c r="N57" t="n">
-        <v>1</v>
-      </c>
-      <c r="O57" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P57" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q57" t="inlineStr">
-        <is>
-          <t xml:space="preserve">EG Experten </t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>HI</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>PSTVA6670</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>PSTVA6670-S2</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>160.63.165.178</t>
-        </is>
-      </c>
-      <c r="H58" t="inlineStr">
-        <is>
-          <t>PSTVA6670</t>
-        </is>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K58" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr"/>
-      <c r="N58" t="n">
-        <v>1</v>
-      </c>
-      <c r="O58" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P58" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q58" t="inlineStr">
-        <is>
-          <t>EG, Expertenraum</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>HI</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>PSTVA6670</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>PSTVA6670-S3</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>160.63.165.178</t>
-        </is>
-      </c>
-      <c r="H59" t="inlineStr">
-        <is>
-          <t>PSTVA6670</t>
-        </is>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K59" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L59" t="inlineStr"/>
-      <c r="N59" t="n">
-        <v>1</v>
-      </c>
-      <c r="O59" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P59" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q59" t="inlineStr">
-        <is>
-          <t>EG, Expertenraum</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>BU</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>PSTVA8670</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>PSTVA8670-S2</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>10.74.17.70</t>
-        </is>
-      </c>
-      <c r="H60" t="inlineStr">
-        <is>
-          <t>PSTVA8670</t>
-        </is>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K60" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr"/>
-      <c r="N60" t="n">
-        <v>1</v>
-      </c>
-      <c r="O60" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P60" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q60" t="inlineStr">
-        <is>
-          <t>EG, Exrpertenbüro</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>BU</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D61" t="inlineStr">
-        <is>
-          <t>PSTVA8670</t>
-        </is>
-      </c>
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>PSTVA8670-S3</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>10.74.17.70</t>
-        </is>
-      </c>
-      <c r="H61" t="inlineStr">
-        <is>
-          <t>PSTVA8670</t>
-        </is>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K61" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr"/>
-      <c r="N61" t="n">
-        <v>1</v>
-      </c>
-      <c r="O61" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P61" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q61" t="inlineStr">
-        <is>
-          <t>EG, Exrpertenbüro</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>GT</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D62" t="inlineStr">
-        <is>
-          <t>PSTVA9670</t>
-        </is>
-      </c>
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>S2</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>PSTVA9670-S2</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>10.74.25.70</t>
-        </is>
-      </c>
-      <c r="H62" t="inlineStr">
-        <is>
-          <t>PSTVA9670</t>
-        </is>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K62" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr"/>
-      <c r="N62" t="n">
-        <v>1</v>
-      </c>
-      <c r="O62" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P62" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q62" t="inlineStr">
-        <is>
-          <t>EG EXPERTENRAUM</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>GT</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>\\vstvacp100001\</t>
-        </is>
-      </c>
-      <c r="D63" t="inlineStr">
-        <is>
-          <t>PSTVA9670</t>
-        </is>
-      </c>
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>S3</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>PSTVA9670-S3</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>10.74.25.70</t>
-        </is>
-      </c>
-      <c r="H63" t="inlineStr">
-        <is>
-          <t>PSTVA9670</t>
-        </is>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>A5</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr">
-        <is>
-          <t>None</t>
-        </is>
-      </c>
-      <c r="L63" t="inlineStr"/>
-      <c r="N63" t="n">
-        <v>1</v>
-      </c>
-      <c r="O63" t="inlineStr">
-        <is>
-          <t>Brother HL-L6250DN</t>
-        </is>
-      </c>
-      <c r="P63" t="inlineStr">
-        <is>
-          <t>Brother HL-6250DN series</t>
-        </is>
-      </c>
-      <c r="Q63" t="inlineStr">
-        <is>
-          <t>EG EXPERTENRAUM</t>
-        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>